<commit_message>
Fixed issues with alchemy and created a command to fix alchemy on the server
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/alchemy-alchemy-skill-increase.xlsx
+++ b/resources/data-imports/Items/alchemy-alchemy-skill-increase.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="112">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
+    <t xml:space="preserve">alchemy_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">specialty_type</t>
   </si>
   <si>
@@ -239,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increases-alchemy-skill</t>
   </si>
   <si>
     <t xml:space="preserve">A simple potion created to give one creativity and inspiration.</t>
@@ -425,13 +431,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -455,83 +465,83 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BS20"/>
+  <dimension ref="A1:BT20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="19" style="1" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="21.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="29.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="38.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="21.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="21.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="20" style="1" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="26.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="38.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="26.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="26.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="26.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="1" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,6 +754,9 @@
       </c>
       <c r="BS1" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,43 +767,43 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>100</v>
+        <v>73</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>100</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1" t="n">
+      <c r="Z2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AD2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH2" s="1" t="n">
-        <v>0</v>
+      <c r="AF2" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI2" s="1" t="n">
         <v>0</v>
@@ -804,32 +817,32 @@
       <c r="AL2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN2" s="1" t="n">
-        <v>1</v>
+      <c r="AM2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR2" s="1" t="n">
-        <v>0</v>
+      <c r="AP2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU2" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW2" s="1" t="n">
-        <v>0.15</v>
       </c>
       <c r="AX2" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="AZ2" s="1" t="n">
-        <v>0</v>
+      <c r="AY2" s="1" t="n">
+        <v>0.15</v>
       </c>
       <c r="BA2" s="1" t="n">
         <v>0</v>
@@ -849,7 +862,7 @@
       <c r="BF2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL2" s="1" t="n">
+      <c r="BG2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM2" s="1" t="n">
@@ -862,6 +875,9 @@
         <v>0</v>
       </c>
       <c r="BP2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -873,43 +889,43 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>200</v>
+      <c r="G3" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>200</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="1" t="n">
+      <c r="Z3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="AD3" s="1" t="n">
+      <c r="AE3" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="AE3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH3" s="1" t="n">
-        <v>0</v>
+      <c r="AF3" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI3" s="1" t="n">
         <v>0</v>
@@ -923,32 +939,32 @@
       <c r="AL3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN3" s="1" t="n">
-        <v>1</v>
+      <c r="AM3" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR3" s="1" t="n">
-        <v>0</v>
+      <c r="AP3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU3" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW3" s="1" t="n">
-        <v>0.1756</v>
       </c>
       <c r="AX3" s="1" t="n">
         <v>0.1756</v>
       </c>
-      <c r="AZ3" s="1" t="n">
-        <v>0</v>
+      <c r="AY3" s="1" t="n">
+        <v>0.1756</v>
       </c>
       <c r="BA3" s="1" t="n">
         <v>0</v>
@@ -968,7 +984,7 @@
       <c r="BF3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL3" s="1" t="n">
+      <c r="BG3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM3" s="1" t="n">
@@ -981,6 +997,9 @@
         <v>0</v>
       </c>
       <c r="BP3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -992,43 +1011,43 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>399</v>
+        <v>73</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>399</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="1" t="n">
+        <v>399</v>
+      </c>
+      <c r="O4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="1" t="n">
+      <c r="Z4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="AD4" s="1" t="n">
+      <c r="AE4" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="AE4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH4" s="1" t="n">
-        <v>0</v>
+      <c r="AF4" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI4" s="1" t="n">
         <v>0</v>
@@ -1042,32 +1061,32 @@
       <c r="AL4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN4" s="1" t="n">
-        <v>1</v>
+      <c r="AM4" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR4" s="1" t="n">
-        <v>0</v>
+      <c r="AP4" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU4" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW4" s="1" t="n">
-        <v>0.2056</v>
       </c>
       <c r="AX4" s="1" t="n">
         <v>0.2056</v>
       </c>
-      <c r="AZ4" s="1" t="n">
-        <v>0</v>
+      <c r="AY4" s="1" t="n">
+        <v>0.2056</v>
       </c>
       <c r="BA4" s="1" t="n">
         <v>0</v>
@@ -1087,7 +1106,7 @@
       <c r="BF4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL4" s="1" t="n">
+      <c r="BG4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM4" s="1" t="n">
@@ -1100,6 +1119,9 @@
         <v>0</v>
       </c>
       <c r="BP4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1111,43 +1133,43 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>795</v>
+        <v>73</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>795</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" s="1" t="n">
+        <v>795</v>
+      </c>
+      <c r="O5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="1" t="n">
+      <c r="Z5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="AD5" s="1" t="n">
+      <c r="AE5" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH5" s="1" t="n">
-        <v>0</v>
+      <c r="AF5" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI5" s="1" t="n">
         <v>0</v>
@@ -1161,32 +1183,32 @@
       <c r="AL5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN5" s="1" t="n">
-        <v>1</v>
+      <c r="AM5" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR5" s="1" t="n">
-        <v>0</v>
+      <c r="AP5" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU5" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW5" s="1" t="n">
-        <v>0.2407</v>
       </c>
       <c r="AX5" s="1" t="n">
         <v>0.2407</v>
       </c>
-      <c r="AZ5" s="1" t="n">
-        <v>0</v>
+      <c r="AY5" s="1" t="n">
+        <v>0.2407</v>
       </c>
       <c r="BA5" s="1" t="n">
         <v>0</v>
@@ -1206,7 +1228,7 @@
       <c r="BF5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL5" s="1" t="n">
+      <c r="BG5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM5" s="1" t="n">
@@ -1219,6 +1241,9 @@
         <v>0</v>
       </c>
       <c r="BP5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1230,43 +1255,43 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>1585</v>
+        <v>73</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>1585</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" s="1" t="n">
+        <v>1585</v>
+      </c>
+      <c r="O6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="1" t="n">
+      <c r="Z6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="AD6" s="1" t="n">
+      <c r="AE6" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="AE6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH6" s="1" t="n">
-        <v>0</v>
+      <c r="AF6" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI6" s="1" t="n">
         <v>0</v>
@@ -1280,32 +1305,32 @@
       <c r="AL6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN6" s="1" t="n">
-        <v>1</v>
+      <c r="AM6" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR6" s="1" t="n">
-        <v>0</v>
+      <c r="AP6" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU6" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW6" s="1" t="n">
-        <v>0.2818</v>
       </c>
       <c r="AX6" s="1" t="n">
         <v>0.2818</v>
       </c>
-      <c r="AZ6" s="1" t="n">
-        <v>0</v>
+      <c r="AY6" s="1" t="n">
+        <v>0.2818</v>
       </c>
       <c r="BA6" s="1" t="n">
         <v>0</v>
@@ -1325,7 +1350,7 @@
       <c r="BF6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL6" s="1" t="n">
+      <c r="BG6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM6" s="1" t="n">
@@ -1338,6 +1363,9 @@
         <v>0</v>
       </c>
       <c r="BP6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1349,43 +1377,43 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>3161</v>
+        <v>73</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>3161</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="1" t="n">
+        <v>3161</v>
+      </c>
+      <c r="O7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="1" t="n">
+      <c r="Z7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="AD7" s="1" t="n">
+      <c r="AE7" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="AE7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH7" s="1" t="n">
-        <v>0</v>
+      <c r="AF7" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI7" s="1" t="n">
         <v>0</v>
@@ -1399,32 +1427,32 @@
       <c r="AL7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN7" s="1" t="n">
-        <v>1</v>
+      <c r="AM7" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR7" s="1" t="n">
-        <v>0</v>
+      <c r="AP7" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU7" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW7" s="1" t="n">
-        <v>0.33</v>
       </c>
       <c r="AX7" s="1" t="n">
         <v>0.33</v>
       </c>
-      <c r="AZ7" s="1" t="n">
-        <v>0</v>
+      <c r="AY7" s="1" t="n">
+        <v>0.33</v>
       </c>
       <c r="BA7" s="1" t="n">
         <v>0</v>
@@ -1444,7 +1472,7 @@
       <c r="BF7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL7" s="1" t="n">
+      <c r="BG7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM7" s="1" t="n">
@@ -1457,6 +1485,9 @@
         <v>0</v>
       </c>
       <c r="BP7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1468,43 +1499,43 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>6305</v>
+        <v>73</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>6305</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" s="1" t="n">
+        <v>6305</v>
+      </c>
+      <c r="O8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="1" t="n">
+      <c r="Z8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="AD8" s="1" t="n">
+      <c r="AE8" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="AE8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH8" s="1" t="n">
-        <v>0</v>
+      <c r="AF8" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI8" s="1" t="n">
         <v>0</v>
@@ -1518,32 +1549,32 @@
       <c r="AL8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN8" s="1" t="n">
-        <v>1</v>
+      <c r="AM8" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR8" s="1" t="n">
-        <v>0</v>
+      <c r="AP8" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU8" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW8" s="1" t="n">
-        <v>0.3863</v>
       </c>
       <c r="AX8" s="1" t="n">
         <v>0.3863</v>
       </c>
-      <c r="AZ8" s="1" t="n">
-        <v>0</v>
+      <c r="AY8" s="1" t="n">
+        <v>0.3863</v>
       </c>
       <c r="BA8" s="1" t="n">
         <v>0</v>
@@ -1563,7 +1594,7 @@
       <c r="BF8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL8" s="1" t="n">
+      <c r="BG8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM8" s="1" t="n">
@@ -1576,6 +1607,9 @@
         <v>0</v>
       </c>
       <c r="BP8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1587,43 +1621,43 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>12600</v>
+        <v>73</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>12600</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" s="1" t="n">
+        <v>12600</v>
+      </c>
+      <c r="O9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="1" t="n">
+      <c r="Z9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="AD9" s="1" t="n">
+      <c r="AE9" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="AE9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH9" s="1" t="n">
-        <v>0</v>
+      <c r="AF9" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI9" s="1" t="n">
         <v>0</v>
@@ -1637,32 +1671,32 @@
       <c r="AL9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN9" s="1" t="n">
-        <v>1</v>
+      <c r="AM9" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR9" s="1" t="n">
-        <v>0</v>
+      <c r="AP9" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU9" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW9" s="1" t="n">
-        <v>0.4523</v>
       </c>
       <c r="AX9" s="1" t="n">
         <v>0.4523</v>
       </c>
-      <c r="AZ9" s="1" t="n">
-        <v>0</v>
+      <c r="AY9" s="1" t="n">
+        <v>0.4523</v>
       </c>
       <c r="BA9" s="1" t="n">
         <v>0</v>
@@ -1682,7 +1716,7 @@
       <c r="BF9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL9" s="1" t="n">
+      <c r="BG9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM9" s="1" t="n">
@@ -1695,6 +1729,9 @@
         <v>0</v>
       </c>
       <c r="BP9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1706,43 +1743,43 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L10" s="1" t="n">
-        <v>25100</v>
+        <v>73</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>25100</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" s="1" t="n">
+        <v>25100</v>
+      </c>
+      <c r="O10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="1" t="n">
+      <c r="Z10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="AD10" s="1" t="n">
+      <c r="AE10" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="AE10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH10" s="1" t="n">
-        <v>0</v>
+      <c r="AF10" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI10" s="1" t="n">
         <v>0</v>
@@ -1756,32 +1793,32 @@
       <c r="AL10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN10" s="1" t="n">
-        <v>1</v>
+      <c r="AM10" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR10" s="1" t="n">
-        <v>0</v>
+      <c r="AP10" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU10" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW10" s="1" t="n">
-        <v>0.5295</v>
       </c>
       <c r="AX10" s="1" t="n">
         <v>0.5295</v>
       </c>
-      <c r="AZ10" s="1" t="n">
-        <v>0</v>
+      <c r="AY10" s="1" t="n">
+        <v>0.5295</v>
       </c>
       <c r="BA10" s="1" t="n">
         <v>0</v>
@@ -1801,7 +1838,7 @@
       <c r="BF10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL10" s="1" t="n">
+      <c r="BG10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM10" s="1" t="n">
@@ -1814,6 +1851,9 @@
         <v>0</v>
       </c>
       <c r="BP10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1825,43 +1865,43 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L11" s="1" t="n">
-        <v>50100</v>
+        <v>73</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>50100</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X11" s="1" t="n">
+        <v>50100</v>
+      </c>
+      <c r="O11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="1" t="n">
+      <c r="Z11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="AD11" s="1" t="n">
+      <c r="AE11" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="AE11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH11" s="1" t="n">
-        <v>0</v>
+      <c r="AF11" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI11" s="1" t="n">
         <v>0</v>
@@ -1875,32 +1915,32 @@
       <c r="AL11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN11" s="1" t="n">
-        <v>1</v>
+      <c r="AM11" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR11" s="1" t="n">
-        <v>0</v>
+      <c r="AP11" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU11" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW11" s="1" t="n">
-        <v>0.62</v>
       </c>
       <c r="AX11" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="AZ11" s="1" t="n">
-        <v>0</v>
+      <c r="AY11" s="1" t="n">
+        <v>0.62</v>
       </c>
       <c r="BA11" s="1" t="n">
         <v>0</v>
@@ -1920,7 +1960,7 @@
       <c r="BF11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL11" s="1" t="n">
+      <c r="BG11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM11" s="1" t="n">
@@ -1933,6 +1973,9 @@
         <v>0</v>
       </c>
       <c r="BP11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1944,43 +1987,43 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L12" s="1" t="n">
-        <v>110500</v>
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>110500</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" s="1" t="n">
+        <v>110500</v>
+      </c>
+      <c r="O12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="1" t="n">
+      <c r="Z12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="AD12" s="1" t="n">
+      <c r="AE12" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="AE12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH12" s="1" t="n">
-        <v>0</v>
+      <c r="AF12" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI12" s="1" t="n">
         <v>0</v>
@@ -1994,32 +2037,32 @@
       <c r="AL12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN12" s="1" t="n">
-        <v>1</v>
+      <c r="AM12" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR12" s="1" t="n">
-        <v>0</v>
+      <c r="AP12" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU12" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW12" s="1" t="n">
-        <v>0.8034</v>
       </c>
       <c r="AX12" s="1" t="n">
         <v>0.8034</v>
       </c>
-      <c r="AZ12" s="1" t="n">
-        <v>0</v>
+      <c r="AY12" s="1" t="n">
+        <v>0.8034</v>
       </c>
       <c r="BA12" s="1" t="n">
         <v>0</v>
@@ -2039,7 +2082,7 @@
       <c r="BF12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL12" s="1" t="n">
+      <c r="BG12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM12" s="1" t="n">
@@ -2052,6 +2095,9 @@
         <v>0</v>
       </c>
       <c r="BP12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2063,43 +2109,43 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L13" s="1" t="n">
-        <v>222800</v>
+        <v>73</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>222800</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" s="1" t="n">
+        <v>222800</v>
+      </c>
+      <c r="O13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="1" t="n">
+      <c r="Z13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="AD13" s="1" t="n">
+      <c r="AE13" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="AE13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH13" s="1" t="n">
-        <v>0</v>
+      <c r="AF13" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI13" s="1" t="n">
         <v>0</v>
@@ -2113,32 +2159,32 @@
       <c r="AL13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN13" s="1" t="n">
-        <v>1</v>
+      <c r="AM13" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR13" s="1" t="n">
-        <v>0</v>
+      <c r="AP13" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU13" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW13" s="1" t="n">
-        <v>0.9502</v>
       </c>
       <c r="AX13" s="1" t="n">
         <v>0.9502</v>
       </c>
-      <c r="AZ13" s="1" t="n">
-        <v>0</v>
+      <c r="AY13" s="1" t="n">
+        <v>0.9502</v>
       </c>
       <c r="BA13" s="1" t="n">
         <v>0</v>
@@ -2158,7 +2204,7 @@
       <c r="BF13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL13" s="1" t="n">
+      <c r="BG13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM13" s="1" t="n">
@@ -2171,6 +2217,9 @@
         <v>0</v>
       </c>
       <c r="BP13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2182,43 +2231,43 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L14" s="1" t="n">
-        <v>449000</v>
+        <v>73</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>449000</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X14" s="1" t="n">
+        <v>449000</v>
+      </c>
+      <c r="O14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="1" t="n">
+      <c r="Z14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="AD14" s="1" t="n">
+      <c r="AE14" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="AE14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH14" s="1" t="n">
-        <v>0</v>
+      <c r="AF14" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI14" s="1" t="n">
         <v>0</v>
@@ -2232,32 +2281,32 @@
       <c r="AL14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN14" s="1" t="n">
-        <v>1</v>
+      <c r="AM14" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR14" s="1" t="n">
-        <v>0</v>
+      <c r="AP14" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU14" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW14" s="1" t="n">
-        <v>1.1238</v>
       </c>
       <c r="AX14" s="1" t="n">
         <v>1.1238</v>
       </c>
-      <c r="AZ14" s="1" t="n">
-        <v>0</v>
+      <c r="AY14" s="1" t="n">
+        <v>1.1238</v>
       </c>
       <c r="BA14" s="1" t="n">
         <v>0</v>
@@ -2277,7 +2326,7 @@
       <c r="BF14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL14" s="1" t="n">
+      <c r="BG14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM14" s="1" t="n">
@@ -2290,6 +2339,9 @@
         <v>0</v>
       </c>
       <c r="BP14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2301,43 +2353,43 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="1" t="n">
-        <v>904900</v>
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>904900</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" s="1" t="n">
+        <v>904900</v>
+      </c>
+      <c r="O15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="1" t="n">
+      <c r="Z15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="AD15" s="1" t="n">
+      <c r="AE15" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="AE15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH15" s="1" t="n">
-        <v>0</v>
+      <c r="AF15" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI15" s="1" t="n">
         <v>0</v>
@@ -2351,32 +2403,32 @@
       <c r="AL15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN15" s="1" t="n">
-        <v>1</v>
+      <c r="AM15" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR15" s="1" t="n">
-        <v>0</v>
+      <c r="AP15" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU15" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW15" s="1" t="n">
-        <v>1.3291</v>
       </c>
       <c r="AX15" s="1" t="n">
         <v>1.3291</v>
       </c>
-      <c r="AZ15" s="1" t="n">
-        <v>0</v>
+      <c r="AY15" s="1" t="n">
+        <v>1.3291</v>
       </c>
       <c r="BA15" s="1" t="n">
         <v>0</v>
@@ -2396,7 +2448,7 @@
       <c r="BF15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL15" s="1" t="n">
+      <c r="BG15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM15" s="1" t="n">
@@ -2409,6 +2461,9 @@
         <v>0</v>
       </c>
       <c r="BP15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2420,43 +2475,43 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L16" s="1" t="n">
-        <v>1823700</v>
+        <v>73</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="M16" s="1" t="n">
         <v>1823700</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X16" s="1" t="n">
+        <v>1823700</v>
+      </c>
+      <c r="O16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC16" s="1" t="n">
+      <c r="Z16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="AD16" s="1" t="n">
+      <c r="AE16" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="AE16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH16" s="1" t="n">
-        <v>0</v>
+      <c r="AF16" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI16" s="1" t="n">
         <v>0</v>
@@ -2470,32 +2525,32 @@
       <c r="AL16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN16" s="1" t="n">
-        <v>1</v>
+      <c r="AM16" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR16" s="1" t="n">
-        <v>0</v>
+      <c r="AP16" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU16" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW16" s="1" t="n">
-        <v>1.572</v>
       </c>
       <c r="AX16" s="1" t="n">
         <v>1.572</v>
       </c>
-      <c r="AZ16" s="1" t="n">
-        <v>0</v>
+      <c r="AY16" s="1" t="n">
+        <v>1.572</v>
       </c>
       <c r="BA16" s="1" t="n">
         <v>0</v>
@@ -2515,7 +2570,7 @@
       <c r="BF16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL16" s="1" t="n">
+      <c r="BG16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM16" s="1" t="n">
@@ -2528,6 +2583,9 @@
         <v>0</v>
       </c>
       <c r="BP16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2539,43 +2597,43 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L17" s="1" t="n">
-        <v>3675300</v>
+        <v>73</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="M17" s="1" t="n">
         <v>3675300</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" s="1" t="n">
+        <v>3675300</v>
+      </c>
+      <c r="O17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="1" t="n">
+      <c r="Z17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="AD17" s="1" t="n">
+      <c r="AE17" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="AE17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH17" s="1" t="n">
-        <v>0</v>
+      <c r="AF17" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI17" s="1" t="n">
         <v>0</v>
@@ -2589,32 +2647,32 @@
       <c r="AL17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN17" s="1" t="n">
-        <v>1</v>
+      <c r="AM17" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR17" s="1" t="n">
-        <v>0</v>
+      <c r="AP17" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU17" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW17" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW17" s="1" t="n">
-        <v>1.8592</v>
       </c>
       <c r="AX17" s="1" t="n">
         <v>1.8592</v>
       </c>
-      <c r="AZ17" s="1" t="n">
-        <v>0</v>
+      <c r="AY17" s="1" t="n">
+        <v>1.8592</v>
       </c>
       <c r="BA17" s="1" t="n">
         <v>0</v>
@@ -2634,7 +2692,7 @@
       <c r="BF17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL17" s="1" t="n">
+      <c r="BG17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM17" s="1" t="n">
@@ -2647,6 +2705,9 @@
         <v>0</v>
       </c>
       <c r="BP17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2658,43 +2719,43 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v>7407100</v>
+        <v>73</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>7407100</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" s="1" t="n">
+        <v>7407100</v>
+      </c>
+      <c r="O18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="1" t="n">
+      <c r="Z18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="AD18" s="1" t="n">
+      <c r="AE18" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="AE18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH18" s="1" t="n">
-        <v>0</v>
+      <c r="AF18" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI18" s="1" t="n">
         <v>0</v>
@@ -2708,32 +2769,32 @@
       <c r="AL18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN18" s="1" t="n">
-        <v>1</v>
+      <c r="AM18" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR18" s="1" t="n">
-        <v>0</v>
+      <c r="AP18" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU18" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW18" s="1" t="n">
-        <v>2.05</v>
       </c>
       <c r="AX18" s="1" t="n">
         <v>2.05</v>
       </c>
-      <c r="AZ18" s="1" t="n">
-        <v>0</v>
+      <c r="AY18" s="1" t="n">
+        <v>2.05</v>
       </c>
       <c r="BA18" s="1" t="n">
         <v>0</v>
@@ -2753,7 +2814,7 @@
       <c r="BF18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL18" s="1" t="n">
+      <c r="BG18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM18" s="1" t="n">
@@ -2766,6 +2827,9 @@
         <v>0</v>
       </c>
       <c r="BP18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2777,43 +2841,43 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L19" s="1" t="n">
-        <v>14928100</v>
+        <v>73</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>14928100</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X19" s="1" t="n">
+        <v>14928100</v>
+      </c>
+      <c r="O19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="1" t="n">
+      <c r="Z19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="AD19" s="1" t="n">
+      <c r="AE19" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="AE19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH19" s="1" t="n">
-        <v>0</v>
+      <c r="AF19" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI19" s="1" t="n">
         <v>0</v>
@@ -2827,32 +2891,32 @@
       <c r="AL19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN19" s="1" t="n">
-        <v>1</v>
+      <c r="AM19" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR19" s="1" t="n">
-        <v>0</v>
+      <c r="AP19" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU19" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW19" s="1" t="n">
-        <v>2.1</v>
       </c>
       <c r="AX19" s="1" t="n">
         <v>2.1</v>
       </c>
-      <c r="AZ19" s="1" t="n">
-        <v>0</v>
+      <c r="AY19" s="1" t="n">
+        <v>2.1</v>
       </c>
       <c r="BA19" s="1" t="n">
         <v>0</v>
@@ -2872,7 +2936,7 @@
       <c r="BF19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL19" s="1" t="n">
+      <c r="BG19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM19" s="1" t="n">
@@ -2887,8 +2951,11 @@
       <c r="BP19" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="BQ19" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
@@ -2896,43 +2963,43 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L20" s="1" t="n">
-        <v>30085500</v>
+        <v>73</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>30085500</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X20" s="1" t="n">
+        <v>30085500</v>
+      </c>
+      <c r="O20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AA20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC20" s="1" t="n">
+      <c r="Z20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="AD20" s="1" t="n">
+      <c r="AE20" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="AE20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH20" s="1" t="n">
-        <v>0</v>
+      <c r="AF20" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="AI20" s="1" t="n">
         <v>0</v>
@@ -2946,32 +3013,32 @@
       <c r="AL20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN20" s="1" t="n">
-        <v>1</v>
+      <c r="AM20" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="AO20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AR20" s="1" t="n">
-        <v>0</v>
+      <c r="AP20" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AS20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="AU20" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="AV20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW20" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AW20" s="1" t="n">
-        <v>2.15</v>
       </c>
       <c r="AX20" s="1" t="n">
         <v>2.15</v>
       </c>
-      <c r="AZ20" s="1" t="n">
-        <v>0</v>
+      <c r="AY20" s="1" t="n">
+        <v>2.15</v>
       </c>
       <c r="BA20" s="1" t="n">
         <v>0</v>
@@ -2991,7 +3058,7 @@
       <c r="BF20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="BL20" s="1" t="n">
+      <c r="BG20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="BM20" s="1" t="n">
@@ -3004,6 +3071,9 @@
         <v>0</v>
       </c>
       <c r="BP20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ20" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>